<commit_message>
Script for RNCS of PU2 Started
</commit_message>
<xml_diff>
--- a/ML/Real_Test.xlsx
+++ b/ML/Real_Test.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\b0612544\Documents\Projects\Quality\ShinyDashboards\RNC_Dashboard\ML\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77E4B485-BA7F-434A-9285-5A80306C4A6C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6BED596-8F91-4990-B125-0A1B1559AF69}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Real_Test" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="52">
   <si>
     <t>Zone</t>
   </si>
@@ -71,24 +71,9 @@
     <t>Methods</t>
   </si>
   <si>
-    <t>Zone 3.2</t>
-  </si>
-  <si>
-    <t>AGX830</t>
-  </si>
-  <si>
     <t>SNC</t>
   </si>
   <si>
-    <t>Zone 3.3</t>
-  </si>
-  <si>
-    <t>AGX950</t>
-  </si>
-  <si>
-    <t>JOINT INSTL, STA 1016, REAR FUSE</t>
-  </si>
-  <si>
     <t>Zone 3.4</t>
   </si>
   <si>
@@ -98,112 +83,112 @@
     <t>Zone 3.1</t>
   </si>
   <si>
-    <t>Q321013840-1</t>
-  </si>
-  <si>
-    <t>AGX806</t>
-  </si>
-  <si>
-    <t>G05361500-003</t>
-  </si>
-  <si>
-    <t>PANEL ASSY, LOWER, AFT FUSE</t>
-  </si>
-  <si>
-    <t>Q321013842-1</t>
-  </si>
-  <si>
-    <t>AGX808</t>
-  </si>
-  <si>
-    <t>G05362500-003</t>
-  </si>
-  <si>
-    <t>PANEL ASSY, RH, AFT FUSE</t>
-  </si>
-  <si>
-    <t>Q321013843-1</t>
-  </si>
-  <si>
-    <t>AGX810</t>
-  </si>
-  <si>
-    <t>Q321013849-1</t>
-  </si>
-  <si>
-    <t>G05365560-104-01</t>
-  </si>
-  <si>
-    <t>ANGLE, SPLICE, UPR, AFT PRESS BHD</t>
-  </si>
-  <si>
-    <t>Q321013837-1</t>
-  </si>
-  <si>
-    <t>G05364500-001-01</t>
-  </si>
-  <si>
-    <t>STRUCTURE ASSY, FUEL TANK, REAR FUSE</t>
-  </si>
-  <si>
-    <t>Q321013809-1</t>
-  </si>
-  <si>
-    <t>G05363921-001</t>
-  </si>
-  <si>
-    <t>Q321013809-2</t>
-  </si>
-  <si>
-    <t>G05530215-101</t>
-  </si>
-  <si>
-    <t>ANGLE, FRONT SPAR, VSTAB</t>
-  </si>
-  <si>
-    <t>Q321013725-3</t>
-  </si>
-  <si>
-    <t>G05450427-101</t>
-  </si>
-  <si>
-    <t>RIB, CTR BOX, PYLON</t>
-  </si>
-  <si>
-    <t>Q321013725-4</t>
-  </si>
-  <si>
-    <t>G05450605-101</t>
-  </si>
-  <si>
     <t>ANGLE, DRAG, CTR BOX, PYLON</t>
   </si>
   <si>
-    <t>METHODS* LOCATION BETWEEN FS 833 &amp; FS 1016, STGR 17 RH &amp; STGR 17 LH, AFFECTED LOWER SKIN, PANEL RH AND LH, IML. ACTUAL CONDITION IS EXIST QTY(20) PARTS WITHOUT THE FINISH CODE REQUIRED BY ENGINEERING DRAWING, PARTS ARE ONLY WITH GREEN COLOR (PRIMER) IN LOWER PANEL G05361500_`003 CONDITION S/B PANEL G05361500_`003 IN IML SIDE SHOULD BE WHITE AS PER FINISH CODE REQUIRED BY DRAWING G00651302, REV D &amp; DRAWING G00651301, REV K IS BAMS 565_`002 (TOPCOAT) PER BAPS 138_`044. PART INSTALLED IN WORK CENTER AGX806 FS 1016 &amp; FS 999 PN SIDE QTY 1. G05379171_`101 LH 1 FS 981 &amp; FS 945 PN SIDE QTY 2. G05362062_`102 LH 1 FS 917 &amp; FS 929 PN SIDE QTY 3. G05361989_`101_`01 LH 1 4. G05361989_`101_`01 RH 1 FS 904 PN SIDE QTY 5. G05361987_`101_`01 LH 1 6. G05361993_`101_`01 LH 1 7. G05361988_`101_`01 RH 1 8. G05361987_`102_`01 RH 1 FS 864 PN SIDE QTY 9. G05361816_`101 LH 1 10. G05361817_`101 LH 1 11. G05379142_`001_`01 LH 1 12. G05361821_`101 LH 1 FS 864 &amp; FS 846 PN SIDE QTY 13. G05361813_`101 _`02 RH 1 FS 846 PN SIDE QTY 14. G05361814_`101 LH 1 15. G05361815_`101 LH 1 16. G05361821_`101 LH 1 17. G05361985_`101_`01 LH 1 18. G05361985_`101_`01 RH 1 19. G05361985_`101_`01 RH 1 20. B0101010AG_`1 RH 1 _`QUERY FOR THIS ISSUE IS #4412 Y #4862 SEE ATTACHMENTS FOR MORE REFERENCES</t>
-  </si>
-  <si>
-    <t>METHODS* LOCATION BETWEEN FS 904 &amp; FS 917, STGR 19 ACTUAL CONDITION IS EXIST QTY(2) PARTS WITHOUT THE FINISH CODE REQUIRED BY ENGINEERING DRAWING G00651302, REV D &amp; DRAWING G00651302, PARTS ONLY HAVE PRIMER. S/B CONDITION FINISH CODE REQUIRED BY DRAWING G00651301 &amp; G00651302 IS BAMS 565_`002 (TOPCOAT) PER BAPS 138_`044. FS 904 &amp; FS 917 1. G05379140_`101 RH 2 _`QUERY FOR THIS ISSUE IS #4412 Y #4862 SEE ATTACHMENTS FOR MORE REFERENCES</t>
-  </si>
-  <si>
-    <t>METHODS* LOCATION BETWEEN FS 833 &amp; FS 1016, STGR 17 RH &amp; STGR 17 LH, AFFECTED LOWER SKIN, PANEL RH AND LH, IML. ACTUAL CONDITION IS EXIST QTY(15) PARTS NUMBERS WITHOUT THE FINISH CODE REQUIRED BY ENGINEERING DRAWING G00651302, REV D &amp; DRAWING G00651302, PARTS ONLY HAVE PRIMER. S/B CONDITION FINISH CODE REQUIRED BY DRAWING G00651301 &amp; G00651302 IS BAMS 565_`002 (TOPCOAT) PER BAPS 138_`044. FS 833 PN SIDE QTY 1. G05362301_`101 RH &amp; LH 2 FS 846 2. G05362821_`101_`01 RH 1 3. G05362034_`101_`01 LH 2 FS 864 4. G05362057_`101 RH 1 5. G05362412_`101 LH 1 FS 881 6. G05362821_`101_`01 LH 1 7. G05379142_`101 LH 2 FS 904 8. G05362822_`101_`01 RH 1 9. G05362038_`102 RH 1 FS 917 10. G05362822_`101_`01 RH 1 11. G05362039_`102 RH 1 FS 929 12. G05362822_`101_`01 RH 1 13. G05362039_`102 RH 1 FS 945 14. G05362822_`101_`01 RH 1 15. G05362090_`102 RH 1 _`QUERY FOR THIS ISSUE IS #4412 Y #4862 SEE ATTACHMENTS FOR MORE REFERENCES</t>
-  </si>
-  <si>
-    <t>METHODS* ANGLE, SPLICE, UPR (G05365560_`104) CONDITION IS NOT FEASIBLE TO USE OR REPAIR. DETAIL STATED AS OBVIOUS SCRAP. IS REQUIRED BY PRODUCTION A NEW B/P PART. SEE ATTACHMENTS FOR DETAILS.</t>
-  </si>
-  <si>
-    <t>METHODS* REFER TO NCR Q320017860, Q320018889, Q320019504, Q321006271, Q321008778 FOR SIMILAR CONDITION ON REPETITIVE ISSUE AFTER SEVERAL TESTS PERFORMED TO PREVENT GAP CONDITION, GAPS WERE FOUND AS FOLLOWS FOR THE TYP 6 LOCATIONS WITH GAP ON STRUCTURE ASSY, FUEL TANK, REAR FUSE (G05364500_`001_`01): _`_`_`_`_`_`_`_`_`_`_`_`_`_`_`_`_`_`_`_`_`_`_`_`_`_`_`_`_`_`_`_`_`_`_`_`_`_`_`_`_`_`_`_`_`_`_`_`_`_`_`_`_`_`_`_`_`_`_`_`_`_`_`_`_`_`_`_`_`_`_`_`_`_`_`_`_`_`_`_`_`_`_`_`_`_`_`_`_`_`_`_`_`_`_`_`_`_`_`_`_`_`_`_`_`_`_`_`_`_`_`_`_`_`_`_`_`_`_`_`_`_`_`_`_`_`_`_`_`_`_`_`_`_`_`_`_`_`_`_`_`_`_`_`_`_`_`_`_`_`_`_`_`_`_`_`_`_`_`_`_`_`_`_`_`_`_`_`_`_`_`_`_`_`_`_`_`_`_`_`_`_`_`_` LOC. INSTL. ENG. DWG. GAP BTWN P/N 1 AND P/N 2, P/N 3 MAX.GAP / LENGTH / WIDTH _`_`_`_`_`_`_`_`_`_`_`_`_`_`_`_`_`_`_`_`_`_`_`_`_`_`_`_`_`_`_`_`_`_`_`_`_`_`_`_`_`_`_`_`_`_`_`_`_`_`_`_`_`_`_`_`_`_`_`_`_`_`_`_`_`_`_`_`_`_`_`_`_`_`_`_`_`_`_`_`_`_`_`_`_`_`_`_`_`_`_`_`_`_`_`_`_`_`_`_`_`_`_`_`_`_`_`_`_`_`_`_`_`_`_`_`_`_`_`_`_`_`_`_`_`_`_`_`_`_`_`_`_`_`_`_`_`_`_`_`_`_`_`_`_`_`_`_`_`_`_`_`_`_`_`_`_`_`_`_`_`_`_`_`_`_`_`_`_`_`_`_`_`_`_`_`_`_`_`_`_`_`_`_` 1 G05364500 REV. H G05364589_`101 G05364545_`101, G05364540_`101 NO GAP FOUND, NO ISSUE 2 G05364500 REV. H G05364588_`101 G05364542_`101 0.010" / 0.630" / 0.160" 3 G05375300 REV. K G05375340_`101 G05364542_`101 0.010" / 0.500" / 0.150" 4 G05375300 REV. K G05375340_`101 G05364542_`102 NO GAP FOUND, NO ISSUE 5 G05364500 REV. H G05364588_`101 G05364542_`102 0.008" / 0.660" / 0.170" 6 G05364500 REV. H G05364589_`102 G05364545_`102, G05364540_`102 NO GAP FOUND, NO ISSUE _`_`_`_`_`_`_`_`_`_`_`_`_`_`_`_`_`_`_`_`_`_`_`_`_`_`_`_`_`_`_`_`_`_`_`_`_`_`_`_`_`_`_`_`_`_`_`_`_`_`_`_`_`_`_`_`_`_`_`_`_`_`_`_`_`_`_`_`_`_`_`_`_`_`_`_`_`_`_`_`_`_`_`_`_`_`_`_`_`_`_`_`_`_`_`_`_`_`_`_`_`_`_`_`_`_`_`_`_`_`_`_`_`_`_`_`_`_`_`_`_`_`_`_`_`_`_`_`_`_`_`_`_`_`_`_`_`_`_`_`_`_`_`_`_`_`_`_`_`_`_`_`_`_`_`_`_`_`_`_`_`_`_`_`_`_`_`_`_`_`_`_`_`_`_`_`_`_`_`_`_`_`_`_` CONSIDER THE FOLLOWING NOTES FOR EVALUATION: _` B/P ON EVERY LOCATION IS MS20470AD5_`*S. _` GAP DOES NOT TOUCH FASTENER SHANK IN ANY LOCATION. _` WHERE NO GAP IN SHOWN, CONSIDER GAP TO BE UNDER 0.005". ALSO, AS MENTIONED ON REFERENCE NCR: THIS IS A REPETITIVE CONDITION USUALLY WITHIN FAYING SURFACE SEAL TOLERANCE (0.005"). WHEN CONDITION EXCEEDS TOLERANCE, GUSSETS ARE REMOVED AND REPLACED WITH OB</t>
-  </si>
-  <si>
-    <t>METHODS* AT FS 1016 UPR THERE ARE QTY 4 EXCESSIVE GAP ON THE ASSY. GAPS WITHOUT APPLYING ANY FORCE (FREE STATE) GAP A RHS A UNIFORM GAP OF .062â IN A LENGTH LENGTH 16â BTWN FITTING, INTERFACE, FRONT SPAR, VS (G05530213_`106) AND SPAR, FRONT, VSTAB (G05530405_`107) GAP B LHS A UNIFORM GAP .062â IN A LENGTH LENGTH 16â BTWN FITTING, INTERFACE, FRONT SPAR, VS (G05530213_`105) AND SPAR, FRONT, VSTAB (G05530405_`109). GAP E LHS A UNIFORM GAP .050â MAX LENGTH 13â BTWN FITTING, INTERFACE, FRONT SPAR, VS (G05530213_`105) AND FRAME, FRONT SPAR (G05363534_`113). Â  GAP F RHS A UNIFORM GAP .050â MAX LENGTH 13â BTWN FITTING, INTERFACE, FRONT SPAR, VS (G05530213_`106) AND FRAME, FRONT SPAR (G05363534_`113). INVOLVED PARTS: FITTING, INTERFACE, FRONT SPAR, VS (G05530213_`106) FITTING, INTERFACE, FRONT SPAR, VS (G05530213_`105) FRAME FROM SPAR (G05363534_`113) SHIM LAMINATED (G05363972_`101) SHIM LAMINATED (G05363973_`101) SPAR, FRONT, VSTAB (G05530405_`109) SEE ATTACHMENTS.</t>
-  </si>
-  <si>
-    <t>METHODS* REF Q320023481_`002. AT FS 1016 BL 0.000 UPR SIDE B/P B0206033AG8 SPAR, FRONT, VSTAB (G05530405_`109) ANGLE, FRONT SPAR, VSTAB (G05530215_`101) EXIST A UNIFORM GAP OF .050" BTWN SPAR AND ANGLE (BETWEEN THE CONTACT SURFACE OF BOTH PIECES) LENGTH: 4.7â WIDTH: 2.9â SEE ATTACHMENTS.</t>
-  </si>
-  <si>
-    <t>METHODS* FS 999, STGR 10, L/H QTY (4) HOLES WITH LOW EDGE DISTANCE CONDITION AT RIB, CTR BOX, PYLON (G05450427_`101) B/P B0205016AD5 PITCH 0.750â COMMON TO: ANGLE, CTR BOX, PYLON (G05450490_`101) ED NOT AN ISSUE SEE ATTACHMENT FOR DETAILS.</t>
-  </si>
-  <si>
-    <t>METHODS* FS 1072, STR 13, LWR CTR BOX PYLON, L/H QTY (1) LOW EDGE DISTANCE CONDITION AT: ANGLE, DRAG, CTR BOX, PYLON (G05450605_`101) ED 0.295â B/P B0205020AD5 PITCH 0.790â COMMON TO: SKIN, LWR, CTR BOX, PYLON (G05450503_`103) ED 0.390" B/P FASTENER IS INSTALLED. SEE ATTACHMENT.</t>
+    <t>Zone 1</t>
+  </si>
+  <si>
+    <t>Q321013865-1</t>
+  </si>
+  <si>
+    <t>AGX744</t>
+  </si>
+  <si>
+    <t>G05372390-001</t>
+  </si>
+  <si>
+    <t>ECS INSTL CPCS PROVISION REAR FUSE</t>
+  </si>
+  <si>
+    <t>Q321013894-1</t>
+  </si>
+  <si>
+    <t>AGX802</t>
+  </si>
+  <si>
+    <t>G05372102-003</t>
+  </si>
+  <si>
+    <t>ECS INSTL TRIM AIR PROVISIONS</t>
+  </si>
+  <si>
+    <t>Q321013725-5</t>
+  </si>
+  <si>
+    <t>G05450606-101</t>
+  </si>
+  <si>
+    <t>Q321013725-6</t>
+  </si>
+  <si>
+    <t>G05361867-102</t>
+  </si>
+  <si>
+    <t>DOUBLER, PYLON, AFT FUSE</t>
+  </si>
+  <si>
+    <t>Q321013727-3</t>
+  </si>
+  <si>
+    <t>G05450605-102</t>
+  </si>
+  <si>
+    <t>Q321013884-1</t>
+  </si>
+  <si>
+    <t>G05360050-005-01</t>
+  </si>
+  <si>
+    <t>CATWALK INSTL, AFT FUSE</t>
+  </si>
+  <si>
+    <t>Zone 4</t>
+  </si>
+  <si>
+    <t>Q321013867-1</t>
+  </si>
+  <si>
+    <t>AGX965</t>
+  </si>
+  <si>
+    <t>G09171071-005</t>
+  </si>
+  <si>
+    <t>CABLE, PWR FDR, ACEPC 1 APU TB RAP</t>
+  </si>
+  <si>
+    <t>Q321013867-2</t>
+  </si>
+  <si>
+    <t>G09171057-007</t>
+  </si>
+  <si>
+    <t>CABLE, PWR FDDR, VFG LHS ACEPC 1 PH A RL</t>
+  </si>
+  <si>
+    <t>METHODS* REFER TO NCR Q321006033. LOCATION: BL0 F.S.897 L/H R/H. EXISTS LOW CLEARANCE CONDITION BETWEEN STIFFENER 1, VERTICAL, AFT PRESS BHD (G05365510_`103) AND TUBE ASSY, CPCS, REAR PRESSURE BULKHEAD (G02193008_`001) AND TUBE ASSY, CPCS, REAR PRESSURE BULKHEAD (G02193007_`001). ACTUAL CONDITION: B/P STANDOFF, TWO LUG, UPRIGHT (B0204034AL_`7W) COMMON TO PART: _` CLAMP, LOOP (M85052/1_`6). _` WASHER, FLAT (B0202033C0332K). _` SCREW, HEX HD (B0201081CK3_`8). LH CLEARANCE = .090" RH CLEARANCE = .090" THE RFC (3000152390) WAS CREATED FOR STANDOFF CHANGE FROM 6 TO 8 LONG BUT CHANGED TO 7 AND THE MINIMUM CLEARANCE SPACE IS NOT AS BAPS 174_`004. A NEW RFC IS REQUIRED. SEE ATTACHMENTS FOR DETAILS REFERENCE RNC Q320003395, Q320004614 AND Q320017825. THE QUERY WAS ALREADY RAISED NO. 542 AND 3356. NOTE: PRODUCTION DECIDED TO INSTALL THE STANDOFF B0204034AL_`8W IN ORDER TO CONTINUE WITH THE PROCESS.</t>
+  </si>
+  <si>
+    <t>METHODS* PARTS INVOLVED P/N. DESCRIPTION. G05364106_`003. BEAM ASSY, FLOOR. G05364101_`003. BEAM ASSY, FLOOR. G05364110_`009. BEAM ASSY, LONGITUDINAL. G05373026_`101. BRACKET, GROUND. REFER TO DRAWING G05372102 REV. _`D, SHEET #2, ZONE 6B, SECTION A_`A FOR BRACKET INSTALLATION. _` B/P FASTENER MS20470AD5_`5S. THE PROCESS TO ACHIEVE THE CONDUCTIVITY BETWEEN BRACKET, GROUND (G05373026_`101) &amp; BEAM ASSY, LONGITUDINAL (G05364110_`009) WAS NOT PERFORMED AS PER WORK INSTRUCTION (GX820502070) &amp; DRAWING REQUIREMENTS (G05372102 REV. _`D) DUE TO THERE IS NOT CONDUCTIVITY BETWEEN COMMON BOLTS (NAS6703A4 AND NAS1149D0332K). ACTUAL CONDITION PROCESS WAS FOLLLOWED ACCORDING TO FINAL DISPOSITION MADE IN NCR Q321007947, Q321008553 &amp; Q321013764 IN ORDER TO ACHIEVE CONDUCTIVITY TOLERANCES AS PER DRAWING (RECORDED VALUE IS LESS OR EQUAL TO 2.5 MILIâ¦) NOTE: PRODUCTION INSTALLED QTY(4) EXTRA BOLTS B0201096V3 WITH QTY_` 4 NAS1149D0332K PER BAPS 150_`000 AND BAPS 150_`002. _` TORQUE APPLIED WAS OF 22.5 LB_`IN. NOTE: METHODS IS WORKING IN RFC SEE ATTACHMENTS FOR REFERENCES</t>
+  </si>
+  <si>
+    <t>METHODS* AT LHS CTR BOX UPR BTWN 1031 AND FS 1016. EXIST QTY 3 DOUBLES HOLES ON ANGLE, DRAG, CTR BOX, PYLON (G05450606_`101). HOLE # 1 B/P B0206002AG5 DIA. DOUBLE HOLE:.164" PITCH:.700" INVOLVED PARTS ANGLE, DRAG, CTR BOX, PYLON (G05450606_`101) E.D: .370" SKIN, SIDE PANEL, AFT BARREL, LH (G05363430_`109) E.D: NOT ISSUE DOUBLER, SIDE PANEL, AFT BARREL, LH (G05363451_`105) E.D: .380" HOLE # 2 B/P B0206002AG5 DIA. DOUBLE HOLE:.164" PITCH:.700" INVOLVED PARTS ANGLE, DRAG, CTR BOX, PYLON (G05450606_`101) E.D: .360" SKIN, SIDE PANEL, AFT BARREL, LH (G05363430_`109) E.D: NOT ISSUE DOUBLER, SIDE PANEL, AFT BARREL, LH (G05363451_`105) E.D: .380" HOLE # 3 B/P B0206002AG5 DIA. DOUBLE HOLE:.167" PITCH:.770" INVOLVED PARTS ANGLE, DRAG, CTR BOX, PYLON (G05450606_`101) E.D: .360" SKIN, SIDE PANEL, AFT BARREL, LH (G05363430_`109) E.D: NOT ISSUE DOUBLER, SIDE PANEL, AFT BARREL, LH (G05363451_`105) E.D: .380" SEE ATTACHMENTS.</t>
+  </si>
+  <si>
+    <t>METHODS* AT RHS CTR BOX UPR BTWN 961 AND FS 981 EXIST QTY 6 HOLES LOW E.D ONLY ON DOUBLER, PYLON, AFT FUSE (G05361867_`102). B/P B0205020AD5 # HOLE DIA. HOLE G&amp;R CKS E.D DRAG E.D DOUBLER 1 .160" .258" .350" .260" 2 .160" .258" .360" .260" 3 .160" .258" .360" .290" 4 .160" .258" .360" .270" 5 .160" .258" .360" .260" 6 .160" .258" .360" .290" INVOLVED PARTS: ANGLE, DRAG, CTR BOX, PYLON (G05450606_`102) SKIN, RH PANEL, AFT FUSE (G05362701_`105) DOUBLER, PYLON, AFT FUSE (G05361867_`102) SEE ATTACHMENTS.</t>
+  </si>
+  <si>
+    <t>METHODS* LOCATION: RHS CTR BOX LWR BTWN 981 AND FS 999 EXIST QTY 4 LOW E.D ONLY ON ANGLE, DRAG, CTR BOX, PYLON (G05450605_`102). B/P B0205020AD5 # HOLE DIA. HOLE ON SKIN DIA. HOLE ON DRAG DIA. HOLE ON FRAME DIA. HOLE ON STR 13 E.D DRAG 1 .160" .098" .098" .098" .290" 2 .130" .098" .098" N/A .280" 3 .130" .098" .098" N/A .280" 4 .130" .098" .098" N/A .250" INVOLVED PARTS: ANGLE, DRAG, CTR BOX, PYLON (G05450605_`102) E.D MIN:.250" SKIN, RH PANEL, AFT FUSE (G05362701_`105) E.D: NOT ISSUE STRINGER 13, AFT FUSE (G05362173_`102) E.D MIN:.360" FRAME, FS999.00, AFT FUSE (G05362370_`106) E.D:.380" SEE ATTACHMENTS.</t>
+  </si>
+  <si>
+    <t>METHOD* DURING INSTALATION AT CATWALK FWD, ASSY G05365001_`001, THERE ARE TAPER GAP CONDITION MAX 0.012", BTWN INTERCOSTAL FWD PANEL, CATWALK (G05365068_`101 AND _`102) AND FRAME, FS981.50 AFT FUSE LOWER STGR 26_`27 LH_`RH. GAP AS FOLLOWS: ZONE A G05365068_`101 TAPER GAP 0.600" _` 0.008â LENGTH 0.700â ZONE B G05365068_`102 TAPER GAP 0.600" _` 0.012" LENGTH 0.600â NOTE RNC REFERENCE Q321002426 SEE THE ATTACHMENT FOR DETAILS</t>
+  </si>
+  <si>
+    <t>METHODS* REFERENCE NCR: 70096 Q321005151 70110 Q321011372 70097 Q321005155 70111 Q321012133 70098 Q321005156 70112 Q321012940 70099 Q321006285 70113 Q321013321 70100 Q321006361 70101 Q321006917 70102 Q321007293 70103 Q321007986 70104 Q321008392 70105 Q321009060 70106 Q321009417 70107 Q321009879 70108 Q321010424 70109 Q321010821 AT FS 1050_`1080, CANTED FRAME LHS, THERE ARE QTY (5) CLAMPS ON HARNESS G09171071_`005 WITH MORE THAN 5 TURNS OF FIBER GLASS TAPE UNDER THE SADDLE CLAMPS, THIS CONDITION DOES NOT MEET THE BAPS 145_`212 (ONLY 5 TURNS ALLOWED) PN: B0305064_`02PH16HC CLAMP, SADDLE QTY 5 SEE ATTACHMENTS AS REFERENCE.</t>
+  </si>
+  <si>
+    <t>METHODS* REFERENCE NCR'S 70096 Q321005151 70110 Q321011372 70097 Q321005155 70111 Q321012133 70098 Q321005156 70112 Q321012940 70098 Q321006285 70113 Q321013321 70100 Q321006361 70101 Q321006917 70102 Q321007293 70103 Q321007986 70104 Q321008392 70105 Q321009060 70106 Q321009417 70107 Q321009879 70108 Q321010424 70109 Q321010821 AT FS 981_`999 STGR 11_`12, LHS AND RHS, THERE ARE QTY (2) SADDLE CLAMPS WITH MORE THAN 5 TURNS OF FIBER GLASS TAPE, THAT CONDITION DOES NOT MEET THE BAPS 145_`212 (MAXIMUM ALLOWED 5 TURNS OF FIBER GLASS TAPE) PN: B0305064_`02PH14HC SADDLE, CLAMP QTY 2 (1 LHS AND 1 RHS) SEE ATTACHMENT AS REFERENCE</t>
   </si>
 </sst>
 </file>
@@ -1049,7 +1034,7 @@
   <dimension ref="A1:J27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7:XFD7"/>
+      <selection activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1092,291 +1077,262 @@
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D2" s="1">
+        <v>44421</v>
+      </c>
+      <c r="E2" t="s">
+        <v>19</v>
+      </c>
+      <c r="F2">
+        <v>70121</v>
+      </c>
+      <c r="G2" t="s">
         <v>20</v>
       </c>
-      <c r="B2" t="s">
+      <c r="H2" t="s">
         <v>21</v>
-      </c>
-      <c r="C2" t="s">
-        <v>14</v>
-      </c>
-      <c r="D2" s="1">
-        <v>44420</v>
-      </c>
-      <c r="E2" t="s">
-        <v>22</v>
-      </c>
-      <c r="F2">
-        <v>70122</v>
-      </c>
-      <c r="G2" t="s">
-        <v>23</v>
-      </c>
-      <c r="H2" t="s">
-        <v>24</v>
       </c>
       <c r="I2" t="s">
         <v>11</v>
       </c>
       <c r="J2" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="B3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3" s="1">
+        <v>44421</v>
+      </c>
+      <c r="E3" t="s">
+        <v>23</v>
+      </c>
+      <c r="F3">
+        <v>70118</v>
+      </c>
+      <c r="G3" t="s">
+        <v>24</v>
+      </c>
+      <c r="H3" t="s">
         <v>25</v>
-      </c>
-      <c r="C3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D3" s="1">
-        <v>44420</v>
-      </c>
-      <c r="E3" t="s">
-        <v>26</v>
-      </c>
-      <c r="F3">
-        <v>70122</v>
-      </c>
-      <c r="G3" t="s">
-        <v>27</v>
-      </c>
-      <c r="H3" t="s">
-        <v>28</v>
       </c>
       <c r="I3" t="s">
         <v>11</v>
       </c>
       <c r="J3" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>20</v>
+        <v>13</v>
       </c>
       <c r="B4" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="C4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D4" s="1">
+        <v>44419</v>
+      </c>
+      <c r="E4" t="s">
         <v>14</v>
       </c>
-      <c r="D4" s="1">
-        <v>44420</v>
-      </c>
-      <c r="E4" t="s">
-        <v>30</v>
-      </c>
       <c r="F4">
-        <v>70122</v>
+        <v>70117</v>
       </c>
       <c r="G4" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="H4" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="I4" t="s">
         <v>11</v>
       </c>
       <c r="J4" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>20</v>
+        <v>13</v>
       </c>
       <c r="B5" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="C5" t="s">
         <v>10</v>
       </c>
       <c r="D5" s="1">
-        <v>44420</v>
+        <v>44419</v>
       </c>
       <c r="E5" t="s">
+        <v>14</v>
+      </c>
+      <c r="F5">
+        <v>70117</v>
+      </c>
+      <c r="G5" t="s">
+        <v>29</v>
+      </c>
+      <c r="H5" t="s">
         <v>30</v>
-      </c>
-      <c r="F5">
-        <v>70120</v>
-      </c>
-      <c r="G5" t="s">
-        <v>32</v>
-      </c>
-      <c r="H5" t="s">
-        <v>33</v>
       </c>
       <c r="I5" t="s">
         <v>11</v>
       </c>
       <c r="J5" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B6" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="C6" t="s">
         <v>10</v>
       </c>
       <c r="D6" s="1">
-        <v>44420</v>
+        <v>44419</v>
       </c>
       <c r="E6" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F6">
-        <v>70116</v>
+        <v>70117</v>
       </c>
       <c r="G6" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="H6" t="s">
-        <v>36</v>
+        <v>16</v>
       </c>
       <c r="I6" t="s">
         <v>11</v>
       </c>
       <c r="J6" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B7" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="C7" t="s">
         <v>10</v>
       </c>
       <c r="D7" s="1">
-        <v>44420</v>
+        <v>44421</v>
       </c>
       <c r="E7" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="F7">
-        <v>70118</v>
+        <v>70116</v>
       </c>
       <c r="G7" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="H7" t="s">
-        <v>17</v>
+        <v>35</v>
       </c>
       <c r="I7" t="s">
         <v>11</v>
       </c>
       <c r="J7" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>15</v>
+        <v>36</v>
       </c>
       <c r="B8" t="s">
+        <v>37</v>
+      </c>
+      <c r="C8" t="s">
+        <v>12</v>
+      </c>
+      <c r="D8" s="1">
+        <v>44421</v>
+      </c>
+      <c r="E8" t="s">
+        <v>38</v>
+      </c>
+      <c r="F8">
+        <v>70114</v>
+      </c>
+      <c r="G8" t="s">
         <v>39</v>
       </c>
-      <c r="C8" t="s">
-        <v>10</v>
-      </c>
-      <c r="D8" s="1">
-        <v>44420</v>
-      </c>
-      <c r="E8" t="s">
-        <v>16</v>
-      </c>
-      <c r="F8">
-        <v>70118</v>
-      </c>
-      <c r="G8" t="s">
+      <c r="H8" t="s">
         <v>40</v>
-      </c>
-      <c r="H8" t="s">
-        <v>41</v>
       </c>
       <c r="I8" t="s">
         <v>11</v>
       </c>
       <c r="J8" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>18</v>
+        <v>36</v>
       </c>
       <c r="B9" t="s">
+        <v>41</v>
+      </c>
+      <c r="C9" t="s">
+        <v>12</v>
+      </c>
+      <c r="D9" s="1">
+        <v>44421</v>
+      </c>
+      <c r="E9" t="s">
+        <v>38</v>
+      </c>
+      <c r="F9">
+        <v>70114</v>
+      </c>
+      <c r="G9" t="s">
         <v>42</v>
       </c>
-      <c r="C9" t="s">
-        <v>10</v>
-      </c>
-      <c r="D9" s="1">
-        <v>44419</v>
-      </c>
-      <c r="E9" t="s">
-        <v>19</v>
-      </c>
-      <c r="F9">
-        <v>70117</v>
-      </c>
-      <c r="G9" t="s">
+      <c r="H9" t="s">
         <v>43</v>
-      </c>
-      <c r="H9" t="s">
-        <v>44</v>
       </c>
       <c r="I9" t="s">
         <v>11</v>
       </c>
       <c r="J9" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>18</v>
-      </c>
-      <c r="B10" t="s">
-        <v>45</v>
-      </c>
-      <c r="C10" t="s">
-        <v>10</v>
-      </c>
-      <c r="D10" s="1">
-        <v>44419</v>
-      </c>
-      <c r="E10" t="s">
-        <v>19</v>
-      </c>
-      <c r="F10">
-        <v>70117</v>
-      </c>
-      <c r="G10" t="s">
-        <v>46</v>
-      </c>
-      <c r="H10" t="s">
-        <v>47</v>
-      </c>
-      <c r="I10" t="s">
-        <v>11</v>
-      </c>
-      <c r="J10" t="s">
-        <v>56</v>
-      </c>
+      <c r="D10" s="1"/>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="D11" s="1"/>

</xml_diff>